<commit_message>
fix(import): repair Item sheet.
</commit_message>
<xml_diff>
--- a/src/import/Nov_21_2016/Item.xlsx
+++ b/src/import/Nov_21_2016/Item.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27904"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="14880" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1120" windowWidth="24960" windowHeight="14880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1778,17 +1779,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -9148,38 +9139,8 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I19">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>[1]Variant!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>I2:I17 I20:I223</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>[1]Category!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H223</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>[1]Origin!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G223</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>[1]Locations!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>J2:J223</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>